<commit_message>
KPI Ticker enhancements as v3.2.0
</commit_message>
<xml_diff>
--- a/documents/Published/KPI Ticker/kpiTickerByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/KPI Ticker/kpiTickerByMAQSoftwareChecklist.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\documents\Published\KPI Ticker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gitlab\documents\Published\KPI Ticker\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053A7BF8-6844-4D1A-AEA5-724F63553ED4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1" xr2:uid="{4AB92824-63E9-41E2-A760-A81835BDCF59}"/>
   </bookViews>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="128">
   <si>
     <t>S no</t>
   </si>
@@ -185,9 +186,6 @@
     <t>Display basic chart</t>
   </si>
   <si>
-    <t>Update text size</t>
-  </si>
-  <si>
     <t>Display default text</t>
   </si>
   <si>
@@ -222,11 +220,6 @@
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>1. Go to formatting pane
-2. Go to Configuration
-3. Update the Size to 40</t>
   </si>
   <si>
     <t>Update Text Color</t>
@@ -248,9 +241,6 @@
     <t xml:space="preserve">3 KPI Columns should be displayed </t>
   </si>
   <si>
-    <t>Configuration</t>
-  </si>
-  <si>
     <t>Indicators</t>
   </si>
   <si>
@@ -279,17 +269,6 @@
   </si>
   <si>
     <t>Indicators should be displayed for all the columns for -1 down arrow with red , for +1 up arrow with green golor and for 0 flat rectangle with blue color</t>
-  </si>
-  <si>
-    <t>Size should be updated to 40</t>
-  </si>
-  <si>
-    <t>1. Go to formatting pane
-2. Go to Configuration
-3. Update Font Color to red</t>
-  </si>
-  <si>
-    <t>Font Color should be updated to red</t>
   </si>
   <si>
     <t>Background color should be updated to sky blue</t>
@@ -328,6 +307,215 @@
 2. Go to Configuration
 3. Update 'KPI Count' value to '3.5'
 </t>
+  </si>
+  <si>
+    <t>1- Go to Formatting pane.                                                                           2- Go to Animation.                                                                                       3- Set duration to 1  second.                                                                      4- Set duration to 5 seconds.</t>
+  </si>
+  <si>
+    <t>Sorting</t>
+  </si>
+  <si>
+    <t>Sort the containers</t>
+  </si>
+  <si>
+    <t>1- Go to Visual's ellipsis menu .                                                                  2-Select the sort by name(or any field).</t>
+  </si>
+  <si>
+    <t>The visual should display containers in the sorted manner on the basis of selected field.</t>
+  </si>
+  <si>
+    <t>Animation on Hover</t>
+  </si>
+  <si>
+    <t>Stop animation on hovering</t>
+  </si>
+  <si>
+    <t>Hover on the visual.</t>
+  </si>
+  <si>
+    <t>Animation should be stopped at the time of hovering on the visual and then start again if not hovered.</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Formatting of KPI</t>
+  </si>
+  <si>
+    <t>Update Text family</t>
+  </si>
+  <si>
+    <t>Font family should be updated to Arial</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to Name
+3. Update Font Color to red</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to Name
+3. Update Font family to Arial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value
+</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to Value
+3. Update Font Color to red</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to Value
+3. Update Font family to Arial</t>
+  </si>
+  <si>
+    <t>Font Color should be updated to Red</t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>1-Go to formatting pane.                                                                                                                                    2- Go to Animation.                                                                                                                                 3-Toggle Horizontal scroll to ON.</t>
+  </si>
+  <si>
+    <t>Ticker should start scrolling in the horizontal manner.</t>
+  </si>
+  <si>
+    <t>1-Go to formatting pane.                                                                              2-Go to Animation.                                                                                          3- Toggle Vertical stack to ON.</t>
+  </si>
+  <si>
+    <t>Ticker's containers should be stacked in vertical manner.</t>
+  </si>
+  <si>
+    <t>1- Go to formatting pane. 
+2- Go to Animation.                                                                                          3- Update style to fade.</t>
+  </si>
+  <si>
+    <t>Update animation style to fade.</t>
+  </si>
+  <si>
+    <t>1- Go to formatting pane. 
+2- Go to Animation.                                                                                          3- Update style to slide and wait.</t>
+  </si>
+  <si>
+    <t>1- Go to formatting pane. 
+2- Go to Animation.                                                                                          3- Update style to no animation.</t>
+  </si>
+  <si>
+    <t>Update style to no animation.</t>
+  </si>
+  <si>
+    <t>Update style to slide and wait.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For duration = 1 second it should be changed to 2 seconds .                For duration = 5 seconds , the Ticker should be on hold for 5 seconds.                </t>
+  </si>
+  <si>
+    <t>Animation style should be changed to fade.
+Change the duration to 5 seconds.
+Ticker should get fade In and fade Out within 5 seconds.</t>
+  </si>
+  <si>
+    <t>There should be no animation.
+Just the data should get replaced with the next data.</t>
+  </si>
+  <si>
+    <t>Animation style should be changed to slide and wait.
+Current data should slide to up or left and next data should get displayed in the same manner respectively.</t>
+  </si>
+  <si>
+    <t>Animation options</t>
+  </si>
+  <si>
+    <t>Scroll the ticker  in horizontal manner.</t>
+  </si>
+  <si>
+    <t>Stack the containers/tickers in the vertical manner.</t>
+  </si>
+  <si>
+    <t>Responsive</t>
+  </si>
+  <si>
+    <t>Make Visual responsive</t>
+  </si>
+  <si>
+    <t>1- Go to Formatting pane.
+2- Go to Responsive.
+3- Toggle Responsive to On.</t>
+  </si>
+  <si>
+    <t>Visual should become responsive i.e. If height and width of the viewport is decreased or increased then the height and width of tiles, wrappers should also get decreased or increased respectively.</t>
+  </si>
+  <si>
+    <t>Set the width of tiles</t>
+  </si>
+  <si>
+    <t>1- Go to Formatting pane.
+2- Go to Responsive.
+3- Toggle Responsive to Off.
+4- Set the width of tiles.</t>
+  </si>
+  <si>
+    <t>Set the height of tiles</t>
+  </si>
+  <si>
+    <t>1- Go to Formatting pane.
+2- Go to Responsive.
+3- Toggle Responsive to Off.
+4- Set the height of tiles.</t>
+  </si>
+  <si>
+    <t>Tiles height should be changed to the value entered in the format option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiles width should be changed to the value entered in the format option. </t>
+  </si>
+  <si>
+    <t>Change alignment</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to Name
+3. Change alignment to Center</t>
+  </si>
+  <si>
+    <t>The tile name should be aligned to center</t>
+  </si>
+  <si>
+    <t>Set duration for animation</t>
+  </si>
+  <si>
+    <t>Carousel</t>
+  </si>
+  <si>
+    <t>Apply Carousel feature</t>
+  </si>
+  <si>
+    <t>1- Go to Formatting pane.
+2- Go to carousel.
+3- Toggle carousel to On.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There should be two arrows according to the scrolling manner selected and clicking on which next/previous data should be appeared without applying animation duration. </t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to Value
+3. Update the Size to 14</t>
+  </si>
+  <si>
+    <t>Size should be updated to 14</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to Name
+3. Update the Size to 14</t>
+  </si>
+  <si>
+    <t>Update text size(Max - 14)</t>
   </si>
 </sst>
 </file>
@@ -440,7 +628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -469,9 +657,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -490,20 +675,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -511,26 +726,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -880,7 +1095,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -891,7 +1106,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -902,7 +1117,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -913,7 +1128,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -924,7 +1139,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -935,7 +1150,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -946,7 +1161,7 @@
         <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -958,7 +1173,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -970,7 +1185,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -981,7 +1196,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3"/>
     </row>
@@ -993,7 +1208,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="3"/>
     </row>
@@ -1005,7 +1220,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="3"/>
     </row>
@@ -1017,33 +1232,33 @@
         <v>14</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+      <c r="A15" s="24">
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="20" t="s">
-        <v>35</v>
+      <c r="C15" s="25" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="25"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="20"/>
+      <c r="C17" s="25"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -1053,46 +1268,46 @@
         <v>18</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
+      <c r="A19" s="24">
         <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>35</v>
+      <c r="C19" s="25" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="20"/>
+      <c r="C20" s="25"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="25"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="20"/>
+      <c r="C22" s="25"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="20"/>
+      <c r="C23" s="25"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -1102,7 +1317,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1113,7 +1328,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1130,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD979CE-A2F4-4A57-BF74-C680FEBF31B0}">
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,558 +1359,978 @@
     <col min="4" max="4" width="55.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="60.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="2" customWidth="1"/>
-    <col min="7" max="16" width="9.140625" style="2"/>
-    <col min="17" max="17" width="9.28515625" style="2" customWidth="1"/>
+    <col min="7" max="14" width="9.140625" style="2"/>
+    <col min="15" max="15" width="8.28515625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" style="2" hidden="1" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+    </row>
+    <row r="3" spans="1:23" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="41">
+        <v>1</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-    </row>
-    <row r="3" spans="1:23" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27">
-        <v>1</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="F3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
+        <v>44</v>
+      </c>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+      <c r="W3" s="27"/>
     </row>
     <row r="4" spans="1:23" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="18" t="s">
+      <c r="A4" s="41"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="27"/>
+    </row>
+    <row r="5" spans="1:23" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="41"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-    </row>
-    <row r="5" spans="1:23" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="18" t="s">
-        <v>61</v>
-      </c>
       <c r="D5" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>62</v>
-      </c>
       <c r="F5" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="21"/>
-    </row>
-    <row r="6" spans="1:23" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+        <v>44</v>
+      </c>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+    </row>
+    <row r="6" spans="1:23" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39">
         <v>2</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>33</v>
+      <c r="B6" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>63</v>
+      <c r="E6" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="F6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+    </row>
+    <row r="7" spans="1:23" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+    </row>
+    <row r="8" spans="1:23" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="39"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="30"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
+    </row>
+    <row r="9" spans="1:23" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+    </row>
+    <row r="10" spans="1:23" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="39"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="26"/>
+      <c r="V10" s="26"/>
+      <c r="W10" s="26"/>
+    </row>
+    <row r="11" spans="1:23" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>3</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="27"/>
+    </row>
+    <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>4</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>5</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>6</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="28"/>
+      <c r="C15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="D15" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16" s="28"/>
+      <c r="C16" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="19"/>
+      <c r="C17" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>7</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-    </row>
-    <row r="7" spans="1:23" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-    </row>
-    <row r="8" spans="1:23" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="9" t="s">
+      <c r="D19" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C20" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>8</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B24" s="38"/>
+      <c r="C24" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B25" s="38"/>
+      <c r="C25" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="22"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-    </row>
-    <row r="9" spans="1:23" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-    </row>
-    <row r="10" spans="1:23" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-    </row>
-    <row r="11" spans="1:23" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
-      <c r="U11" s="22"/>
-      <c r="V11" s="22"/>
-      <c r="W11" s="22"/>
-    </row>
-    <row r="12" spans="1:23" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="22"/>
-      <c r="U12" s="22"/>
-      <c r="V12" s="22"/>
-      <c r="W12" s="22"/>
-    </row>
-    <row r="13" spans="1:23" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
-        <v>3</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
+      <c r="E26" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>9</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B28" s="38"/>
+      <c r="C28" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B29" s="38"/>
+      <c r="C29" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="12">
+        <v>10</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B6:B12"/>
-    <mergeCell ref="A6:A12"/>
+  <mergeCells count="33">
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="R1:W2"/>
-    <mergeCell ref="R3:W3"/>
-    <mergeCell ref="R4:W4"/>
-    <mergeCell ref="J5:Q5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A3:A5"/>
     <mergeCell ref="R5:W5"/>
     <mergeCell ref="J3:Q3"/>
     <mergeCell ref="J1:Q2"/>
     <mergeCell ref="J6:Q6"/>
     <mergeCell ref="R6:W6"/>
-    <mergeCell ref="J7:Q7"/>
+    <mergeCell ref="R1:W2"/>
+    <mergeCell ref="R3:W3"/>
+    <mergeCell ref="R4:W4"/>
+    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="J5:Q5"/>
     <mergeCell ref="R7:W7"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B6:B10"/>
     <mergeCell ref="J8:Q8"/>
     <mergeCell ref="R8:W8"/>
+    <mergeCell ref="J11:Q11"/>
+    <mergeCell ref="R11:W11"/>
+    <mergeCell ref="J10:Q10"/>
+    <mergeCell ref="R10:W10"/>
     <mergeCell ref="J9:Q9"/>
     <mergeCell ref="R9:W9"/>
-    <mergeCell ref="J10:Q10"/>
-    <mergeCell ref="R10:W10"/>
-    <mergeCell ref="J13:Q13"/>
-    <mergeCell ref="R13:W13"/>
-    <mergeCell ref="J12:Q12"/>
-    <mergeCell ref="R12:W12"/>
-    <mergeCell ref="J11:Q11"/>
-    <mergeCell ref="R11:W11"/>
+    <mergeCell ref="J7:Q7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>